<commit_message>
Method Description added and TicketBulkUpdateTest
</commit_message>
<xml_diff>
--- a/resources/excels/TZ.xlsx
+++ b/resources/excels/TZ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34680" windowHeight="11115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34680" windowHeight="11115" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="696">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -1798,21 +1798,6 @@
     <t>Next Reset Date</t>
   </si>
   <si>
-    <t>200121000214</t>
-  </si>
-  <si>
-    <t>200121000215</t>
-  </si>
-  <si>
-    <t>200121000216</t>
-  </si>
-  <si>
-    <t>200121000217</t>
-  </si>
-  <si>
-    <t>200121000218</t>
-  </si>
-  <si>
     <t>QWFpcnRlbEAwOTE5</t>
   </si>
   <si>
@@ -2121,13 +2106,40 @@
   </si>
   <si>
     <t>FnF Indicator</t>
+  </si>
+  <si>
+    <t>Ticket Field 1 - Label</t>
+  </si>
+  <si>
+    <t>Ticket 1 Type</t>
+  </si>
+  <si>
+    <t>Ticket Field 2 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 3 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 4 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 5 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 6 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 7 - Label</t>
+  </si>
+  <si>
+    <t>160621012721</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2227,6 +2239,11 @@
       <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0383F3"/>
+      <name val="Tondo-regular"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2366,7 +2383,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
@@ -2464,6 +2481,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3047,7 +3065,7 @@
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
@@ -3056,7 +3074,7 @@
     <col min="15" max="15" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -3103,44 +3121,44 @@
         <v>14</v>
       </c>
       <c r="P1" s="39" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16.5">
       <c r="A2" s="39">
         <v>2388008</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="C2" t="s">
         <v>463</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="I2" s="54" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="Q2" s="56" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="39">
         <v>2394650</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="C3" t="s">
         <v>464</v>
@@ -3154,31 +3172,31 @@
       </c>
       <c r="Q3" s="39"/>
     </row>
-    <row r="4" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.5">
       <c r="A4" s="39">
         <v>2390932</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="C4" t="s">
         <v>465</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="O4" s="39"/>
       <c r="P4" s="39" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="Q4" s="39"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="39">
         <v>2388008</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="C5" t="s">
         <v>466</v>
@@ -3188,7 +3206,7 @@
       </c>
       <c r="O5" s="39"/>
       <c r="P5" s="39" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="Q5" s="39"/>
     </row>
@@ -3206,14 +3224,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>54</v>
       </c>
@@ -3224,7 +3242,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="11" t="s">
         <v>57</v>
       </c>
@@ -3233,7 +3251,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="12" t="s">
         <v>58</v>
       </c>
@@ -3242,7 +3260,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="12" t="s">
         <v>60</v>
       </c>
@@ -3251,7 +3269,7 @@
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>61</v>
       </c>
@@ -3260,7 +3278,7 @@
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="12" t="s">
         <v>62</v>
       </c>
@@ -3284,13 +3302,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="45" t="s">
         <v>468</v>
       </c>
@@ -3298,7 +3316,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>470</v>
       </c>
@@ -3306,7 +3324,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>472</v>
       </c>
@@ -3314,7 +3332,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>474</v>
       </c>
@@ -3322,17 +3340,17 @@
         <v>475</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>477</v>
       </c>
@@ -3350,7 +3368,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
     <col min="2" max="2" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
@@ -3360,7 +3378,7 @@
     <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
         <v>480</v>
       </c>
@@ -3390,7 +3408,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1" collapsed="1"/>
@@ -3407,7 +3425,7 @@
     <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>509</v>
       </c>
@@ -3448,7 +3466,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="141.75">
       <c r="A2" s="1" t="s">
         <v>522</v>
       </c>
@@ -3490,7 +3508,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.140625" style="1" collapsed="1"/>
@@ -3500,7 +3518,7 @@
     <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="58" t="s">
         <v>486</v>
       </c>
@@ -3523,16 +3541,16 @@
         <v>492</v>
       </c>
       <c r="H1" s="59" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="I1" s="59" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="J1" s="60" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>493</v>
       </c>
@@ -3546,9 +3564,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="58" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="B3" s="58"/>
       <c r="C3" s="58"/>
@@ -3557,19 +3575,19 @@
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
       <c r="H3" s="58" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I3" s="58" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="J3" s="58" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="61"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="58" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="58"/>
@@ -3583,9 +3601,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="58" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B5" s="58"/>
       <c r="C5" s="58"/>
@@ -3599,9 +3617,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="58" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="B6" s="58"/>
       <c r="C6" s="58"/>
@@ -3615,9 +3633,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="58" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B7" s="58"/>
       <c r="C7" s="58"/>
@@ -3631,9 +3649,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="58" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B8" s="58"/>
       <c r="C8" s="58"/>
@@ -3647,9 +3665,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="58" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="B9" s="58"/>
       <c r="C9" s="58"/>
@@ -3663,9 +3681,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="58" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
@@ -3679,9 +3697,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="58" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B11" s="58"/>
       <c r="C11" s="58"/>
@@ -3695,9 +3713,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="58" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="B12" s="58"/>
       <c r="C12" s="58"/>
@@ -3711,9 +3729,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="58" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B13" s="58"/>
       <c r="C13" s="58"/>
@@ -3741,7 +3759,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="63" customWidth="1"/>
     <col min="2" max="2" width="27.140625" style="63" customWidth="1"/>
@@ -3749,163 +3767,163 @@
     <col min="4" max="16384" width="10.85546875" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="62" t="s">
+        <v>632</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>633</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="62" t="s">
+        <v>635</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>636</v>
+      </c>
+      <c r="C2" s="62" t="s">
         <v>637</v>
       </c>
-      <c r="B1" s="62" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="47.25">
+      <c r="A3" s="62" t="s">
         <v>638</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="B3" s="62" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="C3" s="62" t="s">
         <v>640</v>
       </c>
-      <c r="B2" s="62" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="62" t="s">
         <v>641</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="B4" s="62" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="C4" s="62" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="62" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="62" t="s">
         <v>644</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="B5" s="62" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="C5" s="62" t="s">
         <v>646</v>
       </c>
-      <c r="B4" s="62" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="31.5">
+      <c r="A6" s="62" t="s">
         <v>647</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="B6" s="62" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="C6" s="64"/>
+    </row>
+    <row r="7" spans="1:3" ht="47.25">
+      <c r="A7" s="62" t="s">
         <v>649</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B7" s="62" t="s">
         <v>650</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C7" s="62" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+    <row r="8" spans="1:3" ht="47.25">
+      <c r="A8" s="62" t="s">
         <v>652</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B8" s="62" t="s">
         <v>653</v>
       </c>
-      <c r="C6" s="64"/>
-    </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="C8" s="62" t="s">
         <v>654</v>
       </c>
-      <c r="B7" s="62" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="47.25">
+      <c r="A9" s="62" t="s">
         <v>655</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="B9" s="62" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+      <c r="C9" s="62" t="s">
         <v>657</v>
       </c>
-      <c r="B8" s="62" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="47.25">
+      <c r="A10" s="62" t="s">
         <v>658</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="B10" s="62" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
+      <c r="C10" s="62" t="s">
         <v>660</v>
       </c>
-      <c r="B9" s="62" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="47.25">
+      <c r="A11" s="62" t="s">
         <v>661</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="B11" s="62" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="C11" s="62" t="s">
         <v>663</v>
       </c>
-      <c r="B10" s="62" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="47.25">
+      <c r="A12" s="62" t="s">
         <v>664</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="B12" s="62" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="C12" s="62" t="s">
         <v>666</v>
       </c>
-      <c r="B11" s="62" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="15.75">
+      <c r="A13" s="62" t="s">
         <v>667</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="B13" s="62" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="C13" s="64"/>
+    </row>
+    <row r="14" spans="1:3" ht="31.5">
+      <c r="A14" s="62" t="s">
         <v>669</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B14" s="62" t="s">
         <v>670</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C14" s="64"/>
+    </row>
+    <row r="15" spans="1:3" ht="31.5">
+      <c r="A15" s="62" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
+      <c r="B15" s="62" t="s">
         <v>672</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="C15" s="62" t="s">
         <v>673</v>
-      </c>
-      <c r="C13" s="64"/>
-    </row>
-    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
-        <v>674</v>
-      </c>
-      <c r="B14" s="62" t="s">
-        <v>675</v>
-      </c>
-      <c r="C14" s="64"/>
-    </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="62" t="s">
-        <v>676</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>677</v>
-      </c>
-      <c r="C15" s="62" t="s">
-        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -3921,7 +3939,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" style="47" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.140625" style="47" collapsed="1"/>
@@ -3930,7 +3948,7 @@
     <col min="5" max="16384" width="9.140625" style="47" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="46" t="s">
         <v>496</v>
       </c>
@@ -3965,7 +3983,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="15" t="s">
         <v>507</v>
       </c>
@@ -3986,7 +4004,7 @@
       <c r="J2" s="46"/>
       <c r="K2" s="46"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="15" t="s">
         <v>485</v>
       </c>
@@ -4007,7 +4025,7 @@
       <c r="J3" s="46"/>
       <c r="K3" s="46"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="15" t="s">
         <v>508</v>
       </c>
@@ -4042,14 +4060,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="16384" width="10.28515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>483</v>
       </c>
@@ -4057,10 +4075,10 @@
         <v>484</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="15" t="s">
         <v>74</v>
       </c>
@@ -4071,7 +4089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
         <v>72</v>
       </c>
@@ -4082,7 +4100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="15" t="s">
         <v>73</v>
       </c>
@@ -4107,42 +4125,42 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="24" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="24" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="24" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="24" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
         <v>238</v>
       </c>
@@ -4156,11 +4174,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4175,7 +4193,7 @@
     <col min="11" max="11" width="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="39" t="s">
         <v>16</v>
       </c>
@@ -4210,13 +4228,13 @@
         <v>576</v>
       </c>
       <c r="L1" s="39" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="M1" s="39" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="39" t="s">
         <v>72</v>
       </c>
@@ -4243,7 +4261,7 @@
       <c r="L2" s="39"/>
       <c r="M2" s="39"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="39" t="s">
         <v>436</v>
       </c>
@@ -4270,7 +4288,7 @@
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="39" t="s">
         <v>440</v>
       </c>
@@ -4284,7 +4302,7 @@
         <v>441</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F4" s="39" t="s">
         <v>435</v>
@@ -4297,7 +4315,7 @@
       <c r="L4" s="39"/>
       <c r="M4" s="39"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="39" t="s">
         <v>442</v>
       </c>
@@ -4330,7 +4348,7 @@
       <c r="L5" s="39"/>
       <c r="M5" s="39"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="39" t="s">
         <v>448</v>
       </c>
@@ -4355,7 +4373,7 @@
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="39" t="s">
         <v>450</v>
       </c>
@@ -4380,7 +4398,7 @@
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="39" t="s">
         <v>452</v>
       </c>
@@ -4407,7 +4425,7 @@
       <c r="L8" s="39"/>
       <c r="M8" s="39"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="39" t="s">
         <v>455</v>
       </c>
@@ -4434,7 +4452,7 @@
       <c r="L9" s="39"/>
       <c r="M9" s="39"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="52" t="s">
         <v>539</v>
       </c>
@@ -4461,7 +4479,7 @@
       <c r="L10" s="39"/>
       <c r="M10" s="39"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="52" t="s">
         <v>544</v>
       </c>
@@ -4488,7 +4506,7 @@
       <c r="L11" s="39"/>
       <c r="M11" s="39"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="52" t="s">
         <v>550</v>
       </c>
@@ -4519,7 +4537,7 @@
       <c r="L12" s="39"/>
       <c r="M12" s="39"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="39" t="s">
         <v>558</v>
       </c>
@@ -4544,7 +4562,7 @@
       <c r="L13" s="39"/>
       <c r="M13" s="39"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="52" t="s">
         <v>562</v>
       </c>
@@ -4581,7 +4599,7 @@
       <c r="L14" s="39"/>
       <c r="M14" s="39"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="52" t="s">
         <v>567</v>
       </c>
@@ -4612,7 +4630,7 @@
       <c r="L15" s="39"/>
       <c r="M15" s="39"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="52" t="s">
         <v>571</v>
       </c>
@@ -4637,7 +4655,7 @@
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="52" t="s">
         <v>580</v>
       </c>
@@ -4662,21 +4680,21 @@
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="52" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C18" s="52" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F18" s="39" t="s">
         <v>486</v>
@@ -4689,68 +4707,68 @@
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
     </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="45">
       <c r="A19" s="52" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>433</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="F19" s="52" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="G19" s="52" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H19" s="52" t="s">
         <v>434</v>
       </c>
       <c r="I19" s="55" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="K19" s="55" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="L19" s="52" t="s">
         <v>435</v>
       </c>
       <c r="M19" s="52" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="52" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C20" s="39" t="s">
         <v>438</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="G20" s="52" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
@@ -4759,18 +4777,18 @@
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="39" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>583</v>
@@ -4779,30 +4797,30 @@
         <v>460</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="I21" s="39" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="39" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="D22" s="39" t="s">
         <v>583</v>
@@ -4811,7 +4829,7 @@
         <v>460</v>
       </c>
       <c r="F22" s="39" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="G22" s="39" t="s">
         <v>486</v>
@@ -4838,9 +4856,9 @@
       <selection activeCell="AL1" sqref="A1:AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="15.75">
       <c r="A1" s="50" t="s">
         <v>25</v>
       </c>
@@ -4956,7 +4974,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="15.75">
       <c r="A2" s="13" t="s">
         <v>239</v>
       </c>
@@ -5022,7 +5040,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="15.75">
       <c r="A3" s="13" t="s">
         <v>239</v>
       </c>
@@ -5082,7 +5100,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="15.75">
       <c r="A4" s="13" t="s">
         <v>239</v>
       </c>
@@ -5160,7 +5178,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="15.75">
       <c r="A5" s="13" t="s">
         <v>239</v>
       </c>
@@ -5238,7 +5256,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="15.75">
       <c r="A6" s="13" t="s">
         <v>239</v>
       </c>
@@ -5308,7 +5326,7 @@
       <c r="AJ6" s="31"/>
       <c r="AK6" s="31"/>
     </row>
-    <row r="7" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="15.75">
       <c r="A7" s="13" t="s">
         <v>239</v>
       </c>
@@ -5386,7 +5404,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="15.75">
       <c r="A8" s="13" t="s">
         <v>239</v>
       </c>
@@ -5452,7 +5470,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" ht="15.75">
       <c r="A9" s="13" t="s">
         <v>239</v>
       </c>
@@ -5512,7 +5530,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="15.75">
       <c r="A10" s="13" t="s">
         <v>239</v>
       </c>
@@ -5560,7 +5578,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="15.75">
       <c r="A11" s="13" t="s">
         <v>239</v>
       </c>
@@ -5608,7 +5626,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="15.75">
       <c r="A12" s="13" t="s">
         <v>239</v>
       </c>
@@ -5680,7 +5698,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="15.75">
       <c r="A13" s="13" t="s">
         <v>239</v>
       </c>
@@ -5746,7 +5764,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="15.75">
       <c r="A14" s="13" t="s">
         <v>239</v>
       </c>
@@ -5818,7 +5836,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="15.75">
       <c r="A15" s="13" t="s">
         <v>239</v>
       </c>
@@ -5890,7 +5908,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="15.75">
       <c r="A16" s="13" t="s">
         <v>239</v>
       </c>
@@ -5956,7 +5974,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15.75">
       <c r="A17" s="13" t="s">
         <v>239</v>
       </c>
@@ -6022,7 +6040,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15.75">
       <c r="A18" s="13" t="s">
         <v>239</v>
       </c>
@@ -6100,7 +6118,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15.75">
       <c r="A19" s="13" t="s">
         <v>239</v>
       </c>
@@ -6178,7 +6196,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15.75">
       <c r="A20" s="13" t="s">
         <v>239</v>
       </c>
@@ -6244,7 +6262,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15.75">
       <c r="A21" s="13" t="s">
         <v>239</v>
       </c>
@@ -6310,7 +6328,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15.75">
       <c r="A22" s="13" t="s">
         <v>239</v>
       </c>
@@ -6376,7 +6394,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="15.75">
       <c r="A23" s="13" t="s">
         <v>286</v>
       </c>
@@ -6424,7 +6442,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15.75">
       <c r="A24" s="13" t="s">
         <v>286</v>
       </c>
@@ -6472,7 +6490,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15.75">
       <c r="A25" s="13" t="s">
         <v>286</v>
       </c>
@@ -6520,7 +6538,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15.75">
       <c r="A26" s="13" t="s">
         <v>239</v>
       </c>
@@ -6580,7 +6598,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15.75">
       <c r="A27" s="13" t="s">
         <v>295</v>
       </c>
@@ -6646,7 +6664,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15.75">
       <c r="A28" s="13" t="s">
         <v>239</v>
       </c>
@@ -6712,7 +6730,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15.75">
       <c r="A29" s="13" t="s">
         <v>239</v>
       </c>
@@ -6778,7 +6796,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15.75">
       <c r="A30" s="37" t="s">
         <v>295</v>
       </c>
@@ -6818,7 +6836,7 @@
       <c r="AJ30" s="39"/>
       <c r="AK30" s="39"/>
     </row>
-    <row r="31" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15.75">
       <c r="A31" s="13" t="s">
         <v>239</v>
       </c>
@@ -6858,7 +6876,7 @@
       <c r="AJ31" s="39"/>
       <c r="AK31" s="39"/>
     </row>
-    <row r="32" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15.75">
       <c r="A32" s="13" t="s">
         <v>307</v>
       </c>
@@ -6902,7 +6920,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15.75">
       <c r="A33" s="25" t="s">
         <v>307</v>
       </c>
@@ -6946,7 +6964,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15.75">
       <c r="A34" s="25" t="s">
         <v>307</v>
       </c>
@@ -6990,7 +7008,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="15.75">
       <c r="A35" s="25" t="s">
         <v>307</v>
       </c>
@@ -7034,7 +7052,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15.75">
       <c r="A36" s="25" t="s">
         <v>307</v>
       </c>
@@ -7078,7 +7096,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15.75">
       <c r="A37" s="41" t="s">
         <v>307</v>
       </c>
@@ -7118,7 +7136,7 @@
       <c r="AJ37" s="39"/>
       <c r="AK37" s="39"/>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37">
       <c r="A38" s="41" t="s">
         <v>307</v>
       </c>
@@ -7158,7 +7176,7 @@
       <c r="AJ38" s="39"/>
       <c r="AK38" s="39"/>
     </row>
-    <row r="39" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15.75">
       <c r="A39" s="13" t="s">
         <v>307</v>
       </c>
@@ -7198,7 +7216,7 @@
       <c r="AJ39" s="39"/>
       <c r="AK39" s="39"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15.75">
       <c r="A40" s="13" t="s">
         <v>307</v>
       </c>
@@ -7250,7 +7268,7 @@
       <c r="AJ40" s="39"/>
       <c r="AK40" s="39"/>
     </row>
-    <row r="41" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15.75">
       <c r="A41" s="13" t="s">
         <v>295</v>
       </c>
@@ -7322,7 +7340,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15.75">
       <c r="A42" s="13" t="s">
         <v>295</v>
       </c>
@@ -7388,7 +7406,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15.75">
       <c r="A43" s="13" t="s">
         <v>295</v>
       </c>
@@ -7454,7 +7472,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15.75">
       <c r="A44" s="13" t="s">
         <v>295</v>
       </c>
@@ -7526,7 +7544,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15.75">
       <c r="A45" s="13" t="s">
         <v>295</v>
       </c>
@@ -7598,7 +7616,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15.75">
       <c r="A46" s="13" t="s">
         <v>295</v>
       </c>
@@ -7670,7 +7688,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="15.75">
       <c r="A47" s="13" t="s">
         <v>295</v>
       </c>
@@ -7742,7 +7760,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15.75">
       <c r="A48" s="13" t="s">
         <v>295</v>
       </c>
@@ -7790,7 +7808,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15.75">
       <c r="A49" s="13" t="s">
         <v>295</v>
       </c>
@@ -7838,7 +7856,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15.75">
       <c r="A50" s="13" t="s">
         <v>295</v>
       </c>
@@ -7886,7 +7904,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15.75">
       <c r="A51" s="13" t="s">
         <v>295</v>
       </c>
@@ -7930,7 +7948,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" ht="15.75">
       <c r="A52" s="13" t="s">
         <v>295</v>
       </c>
@@ -7974,7 +7992,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15.75">
       <c r="A53" s="13" t="s">
         <v>295</v>
       </c>
@@ -8018,7 +8036,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15.75">
       <c r="A54" s="13" t="s">
         <v>295</v>
       </c>
@@ -8062,7 +8080,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15.75">
       <c r="A55" s="13" t="s">
         <v>295</v>
       </c>
@@ -8106,7 +8124,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15.75">
       <c r="A56" s="13" t="s">
         <v>295</v>
       </c>
@@ -8150,7 +8168,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15.75">
       <c r="A57" s="13" t="s">
         <v>295</v>
       </c>
@@ -8194,7 +8212,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15.75">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -8238,7 +8256,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15.75">
       <c r="A59" s="13" t="s">
         <v>295</v>
       </c>
@@ -8282,7 +8300,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15.75">
       <c r="A60" s="13" t="s">
         <v>295</v>
       </c>
@@ -8326,7 +8344,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" ht="15.75">
       <c r="A61" s="13" t="s">
         <v>295</v>
       </c>
@@ -8370,7 +8388,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="15.75">
       <c r="A62" s="13" t="s">
         <v>295</v>
       </c>
@@ -8418,7 +8436,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15.75">
       <c r="A63" s="13" t="s">
         <v>295</v>
       </c>
@@ -8484,7 +8502,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15.75">
       <c r="A64" s="13" t="s">
         <v>295</v>
       </c>
@@ -8532,7 +8550,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15.75">
       <c r="A65" s="13" t="s">
         <v>295</v>
       </c>
@@ -8598,7 +8616,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15.75">
       <c r="A66" s="13" t="s">
         <v>295</v>
       </c>
@@ -8646,7 +8664,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15.75">
       <c r="A67" s="13" t="s">
         <v>295</v>
       </c>
@@ -8694,7 +8712,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15.75">
       <c r="A68" s="13" t="s">
         <v>295</v>
       </c>
@@ -8742,7 +8760,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15.75">
       <c r="A69" s="13" t="s">
         <v>295</v>
       </c>
@@ -8790,7 +8808,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15.75">
       <c r="A70" s="13" t="s">
         <v>295</v>
       </c>
@@ -8838,7 +8856,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15.75">
       <c r="A71" s="13" t="s">
         <v>295</v>
       </c>
@@ -8886,7 +8904,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15.75">
       <c r="A72" s="13" t="s">
         <v>295</v>
       </c>
@@ -8934,7 +8952,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="15.75">
       <c r="A73" s="13" t="s">
         <v>295</v>
       </c>
@@ -8982,7 +9000,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15.75">
       <c r="A74" s="13" t="s">
         <v>295</v>
       </c>
@@ -9030,7 +9048,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" ht="15.75">
       <c r="A75" s="13" t="s">
         <v>295</v>
       </c>
@@ -9078,7 +9096,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" ht="15.75">
       <c r="A76" s="13" t="s">
         <v>295</v>
       </c>
@@ -9149,15 +9167,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG6"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BA3" sqref="BA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:59" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="15.75">
       <c r="A1" s="50" t="s">
         <v>25</v>
       </c>
@@ -9237,43 +9255,106 @@
         <v>32</v>
       </c>
       <c r="AA1" t="s">
+        <v>687</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>688</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>691</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>692</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>693</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>462</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>694</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AW1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AX1" t="s">
         <v>532</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AY1" t="s">
         <v>533</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AZ1" t="s">
         <v>534</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="BA1" t="s">
         <v>535</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="BB1" t="s">
         <v>536</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="BC1" t="s">
         <v>537</v>
       </c>
-      <c r="AI1" s="51" t="s">
+      <c r="BD1" t="s">
         <v>538</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="BE1" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BF1" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BG1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="15.75">
       <c r="A2" s="13" t="s">
         <v>239</v>
       </c>
@@ -9344,44 +9425,29 @@
       <c r="AL2" s="39" t="s">
         <v>479</v>
       </c>
-      <c r="BG2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="U3" t="s">
-        <v>586</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="U4" t="s">
-        <v>587</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="U5" t="s">
-        <v>588</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="U6" t="s">
-        <v>589</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>589</v>
+      <c r="AV2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW2" s="13">
+        <v>24</v>
+      </c>
+      <c r="BD2">
+        <f>SUM(AW2,AY2,BA2,BC2)</f>
+        <v>24</v>
+      </c>
+      <c r="BE2" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF2" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="BG2" s="65" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9393,7 +9459,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -9403,7 +9469,7 @@
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -9423,7 +9489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
@@ -9440,7 +9506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="21" t="s">
         <v>91</v>
       </c>
@@ -9457,7 +9523,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="21" t="s">
         <v>91</v>
       </c>
@@ -9474,7 +9540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="21" t="s">
         <v>91</v>
       </c>
@@ -9491,7 +9557,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="21" t="s">
         <v>91</v>
       </c>
@@ -9508,7 +9574,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="21" t="s">
         <v>91</v>
       </c>
@@ -9525,7 +9591,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="21" t="s">
         <v>91</v>
       </c>
@@ -9542,7 +9608,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="21" t="s">
         <v>91</v>
       </c>
@@ -9559,7 +9625,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="21" t="s">
         <v>91</v>
       </c>
@@ -9576,7 +9642,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="21" t="s">
         <v>91</v>
       </c>
@@ -9593,7 +9659,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="17" t="s">
         <v>119</v>
       </c>
@@ -9610,7 +9676,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="17" t="s">
         <v>119</v>
       </c>
@@ -9627,7 +9693,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="17" t="s">
         <v>119</v>
       </c>
@@ -9644,7 +9710,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="17" t="s">
         <v>119</v>
       </c>
@@ -9661,7 +9727,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="17" t="s">
         <v>119</v>
       </c>
@@ -9678,7 +9744,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="17" t="s">
         <v>119</v>
       </c>
@@ -9695,7 +9761,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="17" t="s">
         <v>119</v>
       </c>
@@ -9712,7 +9778,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75">
       <c r="A19" s="17" t="s">
         <v>119</v>
       </c>
@@ -9729,7 +9795,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="17" t="s">
         <v>119</v>
       </c>
@@ -9746,7 +9812,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75">
       <c r="A21" s="17" t="s">
         <v>119</v>
       </c>
@@ -9763,7 +9829,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="17" t="s">
         <v>119</v>
       </c>
@@ -9780,7 +9846,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="17" t="s">
         <v>119</v>
       </c>
@@ -9797,7 +9863,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="17" t="s">
         <v>119</v>
       </c>
@@ -9814,7 +9880,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="17" t="s">
         <v>119</v>
       </c>
@@ -9831,7 +9897,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75">
       <c r="A26" s="17" t="s">
         <v>119</v>
       </c>
@@ -9848,7 +9914,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75">
       <c r="A27" s="17" t="s">
         <v>119</v>
       </c>
@@ -9865,7 +9931,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75">
       <c r="A28" s="17" t="s">
         <v>119</v>
       </c>
@@ -9882,7 +9948,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="17" t="s">
         <v>119</v>
       </c>
@@ -9899,7 +9965,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75">
       <c r="A30" s="17" t="s">
         <v>119</v>
       </c>
@@ -9916,7 +9982,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="17" t="s">
         <v>119</v>
       </c>
@@ -9933,7 +9999,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="17" t="s">
         <v>119</v>
       </c>
@@ -9950,7 +10016,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75">
       <c r="A33" s="17" t="s">
         <v>119</v>
       </c>
@@ -9967,7 +10033,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.75">
       <c r="A34" s="17" t="s">
         <v>119</v>
       </c>
@@ -9984,7 +10050,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.75">
       <c r="A35" s="17" t="s">
         <v>119</v>
       </c>
@@ -10001,7 +10067,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75">
       <c r="A36" s="17" t="s">
         <v>119</v>
       </c>
@@ -10018,7 +10084,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75">
       <c r="A37" s="17" t="s">
         <v>119</v>
       </c>
@@ -10035,7 +10101,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="17" t="s">
         <v>119</v>
       </c>
@@ -10052,7 +10118,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.75">
       <c r="A39" s="17" t="s">
         <v>119</v>
       </c>
@@ -10069,7 +10135,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75">
       <c r="A40" s="17" t="s">
         <v>119</v>
       </c>
@@ -10086,7 +10152,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.75">
       <c r="A41" s="17" t="s">
         <v>119</v>
       </c>
@@ -10103,7 +10169,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75">
       <c r="A42" s="17" t="s">
         <v>119</v>
       </c>
@@ -10120,7 +10186,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.75">
       <c r="A43" s="17" t="s">
         <v>119</v>
       </c>
@@ -10137,7 +10203,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.75">
       <c r="A44" s="17" t="s">
         <v>119</v>
       </c>
@@ -10154,7 +10220,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75">
       <c r="A45" s="17" t="s">
         <v>119</v>
       </c>
@@ -10171,7 +10237,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75">
       <c r="A46" s="17" t="s">
         <v>119</v>
       </c>
@@ -10188,7 +10254,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.75">
       <c r="A47" s="17" t="s">
         <v>119</v>
       </c>
@@ -10205,7 +10271,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75">
       <c r="A48" s="17" t="s">
         <v>119</v>
       </c>
@@ -10222,7 +10288,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="17" t="s">
         <v>119</v>
       </c>
@@ -10239,7 +10305,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="17" t="s">
         <v>119</v>
       </c>
@@ -10256,7 +10322,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="17" t="s">
         <v>119</v>
       </c>
@@ -10273,7 +10339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15.75">
       <c r="A52" s="17" t="s">
         <v>119</v>
       </c>
@@ -10290,7 +10356,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="21" t="s">
         <v>91</v>
       </c>
@@ -10307,7 +10373,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15.75">
       <c r="A54" s="17" t="s">
         <v>119</v>
       </c>
@@ -10324,7 +10390,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15.75">
       <c r="A55" s="21" t="s">
         <v>91</v>
       </c>
@@ -10341,7 +10407,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.75">
       <c r="A56" s="17" t="s">
         <v>119</v>
       </c>
@@ -10358,7 +10424,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.75">
       <c r="A57" s="21" t="s">
         <v>91</v>
       </c>
@@ -10375,7 +10441,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.75">
       <c r="A58" s="21" t="s">
         <v>91</v>
       </c>
@@ -10392,7 +10458,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.75">
       <c r="A59" s="17" t="s">
         <v>119</v>
       </c>
@@ -10409,7 +10475,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="21" t="s">
         <v>91</v>
       </c>
@@ -10426,7 +10492,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75">
       <c r="A61" s="21" t="s">
         <v>91</v>
       </c>
@@ -10443,7 +10509,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="17" t="s">
         <v>119</v>
       </c>
@@ -10460,7 +10526,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="17" t="s">
         <v>119</v>
       </c>
@@ -10477,7 +10543,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75">
       <c r="A64" s="17" t="s">
         <v>119</v>
       </c>
@@ -10494,7 +10560,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75">
       <c r="A65" s="17" t="s">
         <v>119</v>
       </c>
@@ -10511,7 +10577,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75">
       <c r="A66" s="17" t="s">
         <v>119</v>
       </c>
@@ -10541,9 +10607,9 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="44" t="s">
         <v>25</v>
       </c>
@@ -10563,7 +10629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
@@ -10580,35 +10646,35 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="20"/>
       <c r="D3" s="18"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="18"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="18"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="18"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -10628,13 +10694,13 @@
       <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="42" t="s">
         <v>53</v>
       </c>
@@ -10645,7 +10711,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="14" t="s">
         <v>63</v>
       </c>
@@ -10656,7 +10722,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="14" t="s">
         <v>64</v>
       </c>
@@ -10667,7 +10733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="14" t="s">
         <v>65</v>
       </c>
@@ -10678,7 +10744,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="14" t="s">
         <v>66</v>
       </c>
@@ -10689,7 +10755,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6" s="15" t="s">
         <v>76</v>
       </c>
@@ -10697,7 +10763,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" s="15" t="s">
         <v>77</v>
       </c>
@@ -10705,7 +10771,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" s="15" t="s">
         <v>78</v>
       </c>
@@ -10713,7 +10779,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9" s="15" t="s">
         <v>79</v>
       </c>
@@ -10721,7 +10787,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" s="15" t="s">
         <v>80</v>
       </c>
@@ -10729,7 +10795,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" s="15" t="s">
         <v>81</v>
       </c>
@@ -10737,7 +10803,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" s="15" t="s">
         <v>82</v>
       </c>
@@ -10745,7 +10811,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" s="15" t="s">
         <v>83</v>
       </c>
@@ -10753,7 +10819,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" s="15" t="s">
         <v>84</v>
       </c>
@@ -10761,7 +10827,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" s="15" t="s">
         <v>85</v>
       </c>
@@ -10769,7 +10835,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" s="15" t="s">
         <v>86</v>
       </c>
@@ -10777,7 +10843,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
@@ -10785,7 +10851,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
@@ -10793,7 +10859,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="16" t="s">
         <v>89</v>
       </c>
@@ -10801,7 +10867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15.75">
       <c r="B20" s="18" t="s">
         <v>90</v>
       </c>
@@ -10822,7 +10888,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -10830,7 +10896,7 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -10844,10 +10910,10 @@
         <v>52</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="43" t="s">
         <v>172</v>
       </c>
@@ -10861,10 +10927,10 @@
         <v>787298771</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="43" t="s">
         <v>478</v>
       </c>
@@ -10878,10 +10944,10 @@
         <v>787298771</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="43" t="s">
         <v>69</v>
       </c>
@@ -10895,7 +10961,7 @@
         <v>787298771</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug FIx related to Recharge History and DA Details
</commit_message>
<xml_diff>
--- a/resources/excels/TZ.xlsx
+++ b/resources/excels/TZ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34680" windowHeight="11115" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34680" windowHeight="11115" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -2523,7 +2523,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2571,7 +2571,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B78FE93F-5E14-564A-B973-EF736B818D9F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B78FE93F-5E14-564A-B973-EF736B818D9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2619,7 +2619,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31D6C7C1-35FA-264C-8C38-CEF3FB365E57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D6C7C1-35FA-264C-8C38-CEF3FB365E57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2667,7 +2667,7 @@
         <xdr:cNvPr id="6" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF7C03D7-7A9D-3140-9B2A-34ADBD00E1C6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7C03D7-7A9D-3140-9B2A-34ADBD00E1C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2715,7 +2715,7 @@
         <xdr:cNvPr id="7" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17E3C7CD-3915-1C46-AC6C-A8CD1CE944E9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17E3C7CD-3915-1C46-AC6C-A8CD1CE944E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2763,7 +2763,7 @@
         <xdr:cNvPr id="8" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BED9E0C-B3A5-A045-9BF7-FA80DDF8A51F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BED9E0C-B3A5-A045-9BF7-FA80DDF8A51F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9169,7 +9169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+    <sheetView topLeftCell="AT1" workbookViewId="0">
       <selection activeCell="BA3" sqref="BA3"/>
     </sheetView>
   </sheetViews>
@@ -10601,10 +10601,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -10645,41 +10645,6 @@
       <c r="E2" s="21" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Changes After 1.15
</commit_message>
<xml_diff>
--- a/resources/excels/TZ.xlsx
+++ b/resources/excels/TZ.xlsx
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="725">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -2655,31 +2655,28 @@
     <t>Any</t>
   </si>
   <si>
+    <t>Customer Number</t>
+  </si>
+  <si>
+    <t>Decorder Number</t>
+  </si>
+  <si>
+    <t>Amount Sent</t>
+  </si>
+  <si>
+    <t>290721013813</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>POSTPAID</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
     <t>New</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>POSTPAID</t>
-  </si>
-  <si>
-    <t>GOLD</t>
-  </si>
-  <si>
-    <t>voice</t>
-  </si>
-  <si>
-    <t>Customer Number</t>
-  </si>
-  <si>
-    <t>Decorder Number</t>
-  </si>
-  <si>
-    <t>Amount Sent</t>
-  </si>
-  <si>
-    <t>280721013807</t>
   </si>
 </sst>
 </file>
@@ -2949,7 +2946,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
@@ -3042,6 +3039,7 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3084,7 +3082,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3132,7 +3130,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B78FE93F-5E14-564A-B973-EF736B818D9F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B78FE93F-5E14-564A-B973-EF736B818D9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3180,7 +3178,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31D6C7C1-35FA-264C-8C38-CEF3FB365E57}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D6C7C1-35FA-264C-8C38-CEF3FB365E57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3228,7 +3226,7 @@
         <xdr:cNvPr id="6" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF7C03D7-7A9D-3140-9B2A-34ADBD00E1C6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF7C03D7-7A9D-3140-9B2A-34ADBD00E1C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3276,7 +3274,7 @@
         <xdr:cNvPr id="7" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17E3C7CD-3915-1C46-AC6C-A8CD1CE944E9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17E3C7CD-3915-1C46-AC6C-A8CD1CE944E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3324,7 +3322,7 @@
         <xdr:cNvPr id="8" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BED9E0C-B3A5-A045-9BF7-FA80DDF8A51F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BED9E0C-B3A5-A045-9BF7-FA80DDF8A51F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10473,7 +10471,7 @@
   <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12780,38 +12778,38 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B77" s="11" t="b">
+      <c r="B77" s="62" t="b">
         <v>0</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="62" t="s">
         <v>714</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E77" s="11" t="s">
-        <v>717</v>
-      </c>
-      <c r="F77" s="11" t="s">
+      <c r="E77" s="62" t="s">
+        <v>724</v>
+      </c>
+      <c r="F77" s="62" t="s">
         <v>713</v>
       </c>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11" t="s">
+      <c r="G77" s="62"/>
+      <c r="H77" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I77" s="11" t="s">
+      <c r="I77" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J77" s="11">
+      <c r="J77" s="62">
         <v>20</v>
       </c>
-      <c r="K77" s="11" t="s">
+      <c r="K77" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L77" s="11">
+      <c r="L77" s="62">
         <v>12</v>
       </c>
       <c r="M77" s="4"/>
@@ -12819,44 +12817,44 @@
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="58">
-        <f t="shared" ref="Q77:Q84" si="2">SUM(L77,J77,N77,P77)</f>
+        <f>SUM(L77,J77,N77,P77)</f>
         <v>32</v>
       </c>
       <c r="R77" s="4"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B78" s="11" t="b">
+      <c r="B78" s="62" t="b">
         <v>0</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="62" t="s">
         <v>714</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D78" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E78" s="11" t="s">
-        <v>718</v>
-      </c>
-      <c r="F78" s="11" t="s">
+      <c r="E78" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="F78" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11" t="s">
+      <c r="G78" s="62"/>
+      <c r="H78" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="I78" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J78" s="11">
+      <c r="J78" s="62">
         <v>18</v>
       </c>
-      <c r="K78" s="11" t="s">
+      <c r="K78" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L78" s="11">
+      <c r="L78" s="62">
         <v>10</v>
       </c>
       <c r="M78" s="4"/>
@@ -12864,44 +12862,44 @@
       <c r="O78" s="4"/>
       <c r="P78" s="4"/>
       <c r="Q78" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L78,J78,N78,P78)</f>
         <v>28</v>
       </c>
       <c r="R78" s="4"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B79" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C79" s="11" t="s">
+      <c r="B79" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="C79" s="62" t="s">
         <v>714</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="E79" s="62" t="s">
         <v>712</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="F79" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11" t="s">
+      <c r="G79" s="62"/>
+      <c r="H79" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I79" s="11" t="s">
+      <c r="I79" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J79" s="11">
+      <c r="J79" s="62">
         <v>15</v>
       </c>
-      <c r="K79" s="11" t="s">
+      <c r="K79" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L79" s="11">
+      <c r="L79" s="62">
         <v>8</v>
       </c>
       <c r="M79" s="4"/>
@@ -12909,44 +12907,44 @@
       <c r="O79" s="4"/>
       <c r="P79" s="4"/>
       <c r="Q79" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L79,J79,N79,P79)</f>
         <v>23</v>
       </c>
       <c r="R79" s="4"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B80" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C80" s="11" t="s">
+      <c r="B80" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="C80" s="62" t="s">
         <v>714</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E80" s="11" t="s">
-        <v>718</v>
-      </c>
-      <c r="F80" s="11" t="s">
+      <c r="E80" s="62" t="s">
+        <v>723</v>
+      </c>
+      <c r="F80" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11" t="s">
+      <c r="G80" s="62"/>
+      <c r="H80" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I80" s="11" t="s">
+      <c r="I80" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J80" s="11">
+      <c r="J80" s="62">
         <v>12</v>
       </c>
-      <c r="K80" s="11" t="s">
+      <c r="K80" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L80" s="11">
+      <c r="L80" s="62">
         <v>6</v>
       </c>
       <c r="M80" s="4"/>
@@ -12954,44 +12952,44 @@
       <c r="O80" s="4"/>
       <c r="P80" s="4"/>
       <c r="Q80" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L80,J80,N80,P80)</f>
         <v>18</v>
       </c>
       <c r="R80" s="4"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B81" s="11" t="b">
+      <c r="B81" s="62" t="b">
         <v>0</v>
       </c>
-      <c r="C81" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D81" s="11" t="s">
+      <c r="C81" s="62" t="s">
+        <v>722</v>
+      </c>
+      <c r="D81" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="E81" s="62" t="s">
         <v>712</v>
       </c>
-      <c r="F81" s="11" t="s">
+      <c r="F81" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11" t="s">
+      <c r="G81" s="62"/>
+      <c r="H81" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I81" s="11" t="s">
+      <c r="I81" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J81" s="11">
+      <c r="J81" s="62">
         <v>18</v>
       </c>
-      <c r="K81" s="11" t="s">
+      <c r="K81" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L81" s="11">
+      <c r="L81" s="62">
         <v>12</v>
       </c>
       <c r="M81" s="4"/>
@@ -12999,44 +12997,44 @@
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
       <c r="Q81" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L81,J81,N81,P81)</f>
         <v>30</v>
       </c>
       <c r="R81" s="4"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B82" s="11" t="b">
+      <c r="B82" s="62" t="b">
         <v>0</v>
       </c>
-      <c r="C82" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D82" s="11" t="s">
+      <c r="C82" s="62" t="s">
+        <v>722</v>
+      </c>
+      <c r="D82" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E82" s="11" t="s">
-        <v>720</v>
-      </c>
-      <c r="F82" s="11" t="s">
+      <c r="E82" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="F82" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11" t="s">
+      <c r="G82" s="62"/>
+      <c r="H82" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I82" s="11" t="s">
+      <c r="I82" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J82" s="11">
+      <c r="J82" s="62">
         <v>15</v>
       </c>
-      <c r="K82" s="11" t="s">
+      <c r="K82" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L82" s="11">
+      <c r="L82" s="62">
         <v>8</v>
       </c>
       <c r="M82" s="4"/>
@@ -13044,44 +13042,44 @@
       <c r="O82" s="4"/>
       <c r="P82" s="4"/>
       <c r="Q82" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L82,J82,N82,P82)</f>
         <v>23</v>
       </c>
       <c r="R82" s="4"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B83" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D83" s="11" t="s">
+      <c r="B83" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="C83" s="62" t="s">
+        <v>722</v>
+      </c>
+      <c r="D83" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E83" s="62" t="s">
         <v>712</v>
       </c>
-      <c r="F83" s="11" t="s">
+      <c r="F83" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11" t="s">
+      <c r="G83" s="62"/>
+      <c r="H83" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I83" s="11" t="s">
+      <c r="I83" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J83" s="11">
+      <c r="J83" s="62">
         <v>12</v>
       </c>
-      <c r="K83" s="11" t="s">
+      <c r="K83" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L83" s="11">
+      <c r="L83" s="62">
         <v>6</v>
       </c>
       <c r="M83" s="4"/>
@@ -13089,44 +13087,44 @@
       <c r="O83" s="4"/>
       <c r="P83" s="4"/>
       <c r="Q83" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L83,J83,N83,P83)</f>
         <v>18</v>
       </c>
       <c r="R83" s="4"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="B84" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D84" s="11" t="s">
+      <c r="B84" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="C84" s="62" t="s">
+        <v>722</v>
+      </c>
+      <c r="D84" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="E84" s="11" t="s">
-        <v>720</v>
-      </c>
-      <c r="F84" s="11" t="s">
+      <c r="E84" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="F84" s="62" t="s">
         <v>716</v>
       </c>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11" t="s">
+      <c r="G84" s="62"/>
+      <c r="H84" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I84" s="11" t="s">
+      <c r="I84" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="J84" s="11">
+      <c r="J84" s="62">
         <v>10</v>
       </c>
-      <c r="K84" s="11" t="s">
+      <c r="K84" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="L84" s="11">
+      <c r="L84" s="62">
         <v>4</v>
       </c>
       <c r="M84" s="4"/>
@@ -13134,7 +13132,7 @@
       <c r="O84" s="4"/>
       <c r="P84" s="4"/>
       <c r="Q84" s="58">
-        <f t="shared" si="2"/>
+        <f>SUM(L84,J84,N84,P84)</f>
         <v>14</v>
       </c>
       <c r="R84" s="4"/>
@@ -13179,7 +13177,7 @@
       <c r="O85" s="4"/>
       <c r="P85" s="4"/>
       <c r="Q85" s="58">
-        <f t="shared" ref="Q85" si="3">SUM(L85,J85,N85,P85)</f>
+        <f t="shared" ref="Q85" si="2">SUM(L85,J85,N85,P85)</f>
         <v>12</v>
       </c>
       <c r="R85" s="4"/>
@@ -13203,7 +13201,7 @@
   <dimension ref="A1:BC2"/>
   <sheetViews>
     <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2"/>
+      <selection activeCell="AP19" sqref="AP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13410,7 +13408,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="58" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="M2" s="22" t="s">
         <v>400</v>
@@ -13419,7 +13417,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="P2" s="22" t="s">
         <v>400</v>
@@ -13428,7 +13426,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="S2" s="22" t="s">
         <v>400</v>
@@ -13482,10 +13480,10 @@
         <v>714</v>
       </c>
       <c r="BB2" s="58" t="s">
-        <v>721</v>
+        <v>62</v>
       </c>
       <c r="BC2" s="58" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>